<commit_message>
ExcelUtility introduced, new methods added.
</commit_message>
<xml_diff>
--- a/TestNG/testData/ExelenterEmployeesList.xlsx
+++ b/TestNG/testData/ExelenterEmployeesList.xlsx
@@ -1,34 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/TestNGProject/testData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA457C23-EB84-5040-81B3-5C88A74157F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-18020" yWindow="-16700" windowWidth="26040" windowHeight="13980" xr2:uid="{7A12BD58-98C9-E048-8107-5573E8AB6C07}"/>
+    <workbookView windowWidth="29920" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -53,24 +34,33 @@
     <t>Adams</t>
   </si>
   <si>
+    <t>willadams12a</t>
+  </si>
+  <si>
+    <t>willAdam_@2023</t>
+  </si>
+  <si>
     <t>Elizabeth</t>
   </si>
   <si>
     <t>Lee</t>
   </si>
   <si>
+    <t>elizabethlee12a</t>
+  </si>
+  <si>
     <t>eliLee_@2023</t>
   </si>
   <si>
-    <t>willAdam_@2023</t>
-  </si>
-  <si>
     <t>Tyler</t>
   </si>
   <si>
     <t>Nguyen</t>
   </si>
   <si>
+    <t>tylernguyen12a</t>
+  </si>
+  <si>
     <t>tylerNguyen_@2023</t>
   </si>
   <si>
@@ -80,31 +70,28 @@
     <t>Smith</t>
   </si>
   <si>
+    <t>johnSmith12a</t>
+  </si>
+  <si>
     <t>johnSmith_@2023!!!</t>
-  </si>
-  <si>
-    <t>willadams12</t>
-  </si>
-  <si>
-    <t>elizabethlee12</t>
-  </si>
-  <si>
-    <t>tylernguyen12</t>
-  </si>
-  <si>
-    <t>johnSmith12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -112,13 +99,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -126,19 +107,348 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -146,28 +456,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -216,7 +808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -249,26 +841,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -301,23 +876,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -459,32 +1017,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57988F14-CEFA-C548-B8A8-EA00BB470A14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.8" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1617647058824" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.2" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +1051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="17" customHeight="1" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -506,60 +1059,60 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="19" customHeight="1" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{413597BE-98BF-C14F-833A-251922B7289F}"/>
+    <hyperlink ref="D5" r:id="rId1" display="johnSmith_@2023!!!"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>